<commit_message>
Commit atualizacao tesouro 23/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -281,7 +281,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,6 +383,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -757,8 +760,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1890050192"/>
-        <c:axId val="-1890046384"/>
+        <c:axId val="-364704256"/>
+        <c:axId val="-364693376"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -891,28 +894,28 @@
                       <c:formatCode>m/d/yyyy</c:formatCode>
                       <c:ptCount val="8"/>
                       <c:pt idx="0" formatCode="0.00">
-                        <c:v>0.37254651083455215</c:v>
+                        <c:v>0.37258862690373018</c:v>
                       </c:pt>
                       <c:pt idx="1" formatCode="0.00">
-                        <c:v>0.37297883012427957</c:v>
+                        <c:v>0.3730209950667891</c:v>
                       </c:pt>
                       <c:pt idx="2" formatCode="0.00">
-                        <c:v>0.37119894265971537</c:v>
+                        <c:v>0.37124090638744661</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
-                        <c:v>0.37129376190375712</c:v>
+                        <c:v>0.37133573635072403</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
-                        <c:v>0.37281320326793688</c:v>
+                        <c:v>0.37285534948646981</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00">
-                        <c:v>0.37384361561003238</c:v>
+                        <c:v>0.37388587831581249</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
-                        <c:v>0.37318607075842564</c:v>
+                        <c:v>0.37322825912931429</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
-                        <c:v>0.37197022094708199</c:v>
+                        <c:v>0.37201227186717378</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -926,7 +929,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -1083,7 +1086,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890050192"/>
+        <c:axId val="-364704256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1129,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890046384"/>
+        <c:crossAx val="-364693376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1134,7 +1137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890046384"/>
+        <c:axId val="-364693376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1188,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890050192"/>
+        <c:crossAx val="-364704256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1621,8 +1624,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1890049648"/>
-        <c:axId val="-1890040944"/>
+        <c:axId val="-364703712"/>
+        <c:axId val="-364702080"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1790,7 +1793,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -1947,7 +1950,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890049648"/>
+        <c:axId val="-364703712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +1993,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890040944"/>
+        <c:crossAx val="-364702080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1998,7 +2001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890040944"/>
+        <c:axId val="-364702080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,7 +2052,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890049648"/>
+        <c:crossAx val="-364703712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3300,6 +3303,7 @@
       <sheetName val="200519"/>
       <sheetName val="210519"/>
       <sheetName val="220519"/>
+      <sheetName val="230519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -3336,6 +3340,7 @@
       <sheetData sheetId="17" refreshError="1"/>
       <sheetData sheetId="18" refreshError="1"/>
       <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3360,6 +3365,7 @@
       <sheetName val="200519"/>
       <sheetName val="210519"/>
       <sheetName val="220519"/>
+      <sheetName val="230519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -3391,18 +3397,19 @@
       <sheetData sheetId="13" refreshError="1"/>
       <sheetData sheetId="14" refreshError="1"/>
       <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16">
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17" refreshError="1"/>
       <sheetData sheetId="18" refreshError="1"/>
       <sheetData sheetId="19" refreshError="1"/>
       <sheetData sheetId="20" refreshError="1"/>
       <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3781,8 +3788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,6 +3813,8 @@
     <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3861,11 +3870,15 @@
       <c r="R1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="T1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="V1" s="22"/>
       <c r="W1" s="22"/>
       <c r="X1" s="22"/>
@@ -3932,11 +3945,15 @@
       <c r="R2" s="15">
         <v>43607</v>
       </c>
-      <c r="S2" s="16">
+      <c r="S2" s="17">
         <v>43607</v>
       </c>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
+      <c r="T2" s="15">
+        <v>43608</v>
+      </c>
+      <c r="U2" s="16">
+        <v>43608</v>
+      </c>
       <c r="V2" s="22"/>
       <c r="W2" s="22"/>
       <c r="X2" s="22"/>
@@ -4007,11 +4024,15 @@
       <c r="R3" s="20">
         <v>4.09</v>
       </c>
-      <c r="S3" s="21">
+      <c r="S3" s="26">
         <v>2618.15</v>
       </c>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
+      <c r="T3" s="20">
+        <v>4.13</v>
+      </c>
+      <c r="U3" s="21">
+        <v>2613.5700000000002</v>
+      </c>
       <c r="V3" s="22"/>
       <c r="W3" s="22"/>
       <c r="X3" s="22"/>
@@ -4082,8 +4103,14 @@
       <c r="R4" s="37">
         <v>3.97</v>
       </c>
-      <c r="S4" s="33">
+      <c r="S4" s="32">
         <v>2633.96</v>
+      </c>
+      <c r="T4" s="37">
+        <v>4.01</v>
+      </c>
+      <c r="U4" s="33">
+        <v>2629.33</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -4091,15 +4118,15 @@
         <v>15</v>
       </c>
       <c r="B5" s="34">
-        <f>B6+S5</f>
-        <v>973.87383397260271</v>
+        <f>B6+U5</f>
+        <v>973.98392958904105</v>
       </c>
       <c r="C5" s="35">
         <v>43598</v>
       </c>
       <c r="D5" s="36">
         <f>$B$5/E3</f>
-        <v>0.37254651083455215</v>
+        <v>0.37258862690373018</v>
       </c>
       <c r="E5" s="38">
         <f>((D3/365)*$B$6)/100</f>
@@ -4107,59 +4134,67 @@
       </c>
       <c r="F5" s="36">
         <f>$B$5/G3</f>
-        <v>0.37297883012427957</v>
+        <v>0.3730209950667891</v>
       </c>
       <c r="G5" s="38">
         <f>(((F3/365)*$B$6)/100)+E5</f>
         <v>0.21832520547945206</v>
       </c>
       <c r="H5" s="36">
-        <f t="shared" ref="H5:S5" si="0">$B$5/I3</f>
-        <v>0.37119894265971537</v>
+        <f t="shared" ref="H5" si="0">$B$5/I3</f>
+        <v>0.37124090638744661</v>
       </c>
       <c r="I5" s="38">
         <f t="shared" ref="I5:I6" si="1">(((H3/365)*$B$6)/100)+G5</f>
         <v>0.32548849315068495</v>
       </c>
       <c r="J5" s="36">
-        <f t="shared" ref="J5:S5" si="2">$B$5/K3</f>
-        <v>0.37129376190375712</v>
+        <f t="shared" ref="J5" si="2">$B$5/K3</f>
+        <v>0.37133573635072403</v>
       </c>
       <c r="K5" s="38">
         <f t="shared" ref="K5:K6" si="3">(((J3/365)*$B$6)/100)+I5</f>
         <v>0.43291835616438357</v>
       </c>
       <c r="L5" s="36">
-        <f t="shared" ref="L5:S5" si="4">$B$5/M3</f>
-        <v>0.37281320326793688</v>
+        <f t="shared" ref="L5" si="4">$B$5/M3</f>
+        <v>0.37285534948646981</v>
       </c>
       <c r="M5" s="38">
         <f t="shared" ref="M5:M6" si="5">(((L3/365)*$B$6)/100)+K5</f>
         <v>0.54274739726027399</v>
       </c>
       <c r="N5" s="36">
-        <f t="shared" ref="N5:S5" si="6">$B$5/O3</f>
-        <v>0.37384361561003238</v>
+        <f t="shared" ref="N5" si="6">$B$5/O3</f>
+        <v>0.37388587831581249</v>
       </c>
       <c r="O5" s="38">
         <f t="shared" ref="O5:O6" si="7">(((N3/365)*$B$6)/100)+M5</f>
         <v>0.65417589041095892</v>
       </c>
       <c r="P5" s="36">
-        <f t="shared" ref="P5:S5" si="8">$B$5/Q3</f>
-        <v>0.37318607075842564</v>
+        <f t="shared" ref="P5" si="8">$B$5/Q3</f>
+        <v>0.37322825912931429</v>
       </c>
       <c r="Q5" s="38">
         <f t="shared" ref="Q5:Q6" si="9">(((P3/365)*$B$6)/100)+O5</f>
         <v>0.76480465753424665</v>
       </c>
       <c r="R5" s="36">
-        <f t="shared" ref="R5:S5" si="10">$B$5/S3</f>
-        <v>0.37197022094708199</v>
+        <f t="shared" ref="R5" si="10">$B$5/S3</f>
+        <v>0.37201227186717378</v>
       </c>
       <c r="S5" s="38">
         <f t="shared" ref="S5:S6" si="11">(((R3/365)*$B$6)/100)+Q5</f>
         <v>0.87383397260273976</v>
+      </c>
+      <c r="T5" s="36">
+        <f t="shared" ref="T5" si="12">$B$5/U3</f>
+        <v>0.37266418331593987</v>
+      </c>
+      <c r="U5" s="38">
+        <f t="shared" ref="U5:U6" si="13">(((T3/365)*$B$6)/100)+S5</f>
+        <v>0.98392958904109595</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -4189,7 +4224,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="36">
-        <f t="shared" ref="H6:S6" si="12">$B$6/I4</f>
+        <f t="shared" ref="H6" si="14">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="38">
@@ -4197,7 +4232,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="36">
-        <f t="shared" ref="J6:S6" si="13">$B$6/K4</f>
+        <f t="shared" ref="J6" si="15">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="38">
@@ -4205,7 +4240,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="36">
-        <f t="shared" ref="L6:S6" si="14">$B$6/M4</f>
+        <f t="shared" ref="L6" si="16">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="38">
@@ -4213,7 +4248,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="36">
-        <f t="shared" ref="N6:S6" si="15">$B$6/O4</f>
+        <f t="shared" ref="N6" si="17">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="38">
@@ -4221,7 +4256,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="36">
-        <f t="shared" ref="P6:S6" si="16">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="18">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="38">
@@ -4229,15 +4264,21 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="36">
-        <f t="shared" ref="R6:S6" si="17">$B$6/S4</f>
+        <f t="shared" ref="R6" si="19">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="38">
         <f t="shared" si="11"/>
         <v>0.84824273972602748</v>
       </c>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
+      <c r="T6" s="36">
+        <f t="shared" ref="T6" si="20">$B$6/U4</f>
+        <v>0.37005625007131093</v>
+      </c>
+      <c r="U6" s="38">
+        <f t="shared" si="13"/>
+        <v>0.95513945205479467</v>
+      </c>
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 27/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -487,13 +487,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -524,6 +524,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -555,6 +558,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -566,14 +572,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$W$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3)</c:f>
+              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>4.08</c:v>
                 </c:pt>
@@ -603,6 +609,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,13 +661,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -689,6 +698,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -720,6 +732,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -731,14 +746,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$W$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4)</c:f>
+              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.96</c:v>
                 </c:pt>
@@ -768,6 +783,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,8 +802,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-109178752"/>
-        <c:axId val="-109168960"/>
+        <c:axId val="1635059952"/>
+        <c:axId val="1635061584"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -838,15 +856,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -877,6 +895,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -908,6 +929,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -919,16 +943,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$W$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.37258862690373018</c:v>
                       </c:pt>
@@ -958,6 +982,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
                         <c:v>0.37119704622471933</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="0.00">
+                        <c:v>0.37080982913114896</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -971,7 +998,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -1015,15 +1042,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1054,6 +1081,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1085,6 +1115,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1096,16 +1129,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$W$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.36996619733304947</c:v>
                       </c:pt>
@@ -1135,6 +1168,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
                         <c:v>0.36859969996817848</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="0.00">
+                        <c:v>0.36821610084504275</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1146,7 +1182,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-109178752"/>
+        <c:axId val="1635059952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1225,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-109168960"/>
+        <c:crossAx val="1635061584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1197,7 +1233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-109168960"/>
+        <c:axId val="1635061584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1284,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-109178752"/>
+        <c:crossAx val="1635059952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,7 +1428,6 @@
                   <c:v>VENDA</c:v>
                 </c:pt>
               </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1424,13 +1459,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1461,6 +1496,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1492,6 +1530,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1503,14 +1544,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$W$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3)</c:f>
+              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2614.1</c:v>
                 </c:pt>
@@ -1540,6 +1581,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2623.9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2626.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1558,7 +1602,6 @@
                   <c:v>COMPRA</c:v>
                 </c:pt>
               </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1590,13 +1633,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1627,6 +1670,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1658,6 +1704,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1669,14 +1718,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$W$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2629.97</c:v>
                 </c:pt>
@@ -1706,6 +1755,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2639.72</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2642.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1722,8 +1774,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-109172768"/>
-        <c:axId val="-109170048"/>
+        <c:axId val="1635062128"/>
+        <c:axId val="1635053424"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1776,15 +1828,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1815,6 +1867,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1846,6 +1901,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1857,16 +1915,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$W$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.1087627397260274</c:v>
                       </c:pt>
@@ -1896,6 +1954,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.0921591780821918</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.1998556164383563</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1953,15 +2014,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1992,6 +2053,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2023,6 +2087,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2034,16 +2101,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$W$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.10556383561643835</c:v>
                       </c:pt>
@@ -2073,6 +2140,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.0601701369863015</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.1646676712328767</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2084,7 +2154,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-109172768"/>
+        <c:axId val="1635062128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2197,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-109170048"/>
+        <c:crossAx val="1635053424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2135,7 +2205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-109170048"/>
+        <c:axId val="1635053424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2256,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-109172768"/>
+        <c:crossAx val="1635062128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2361,13 +2431,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2398,6 +2468,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2429,6 +2502,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2440,14 +2516,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$W$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5)</c:f>
+              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.37258862690373018</c:v>
                 </c:pt>
@@ -2477,6 +2553,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>0.37119704622471933</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.37080982913114896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2526,13 +2605,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2563,6 +2642,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2594,6 +2676,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2605,14 +2690,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$W$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.36996619733304947</c:v>
                 </c:pt>
@@ -2642,6 +2727,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>0.36859969996817848</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.36821610084504275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2658,8 +2746,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2037064336"/>
-        <c:axId val="-2037067600"/>
+        <c:axId val="1635062672"/>
+        <c:axId val="1635051792"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2712,15 +2800,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2751,6 +2839,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2782,6 +2873,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2793,16 +2887,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$W$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>4.08</c:v>
                       </c:pt>
@@ -2832,6 +2926,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.0599999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.04</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2889,15 +2986,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2928,6 +3025,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2959,6 +3059,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2970,16 +3073,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$W$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>3.96</c:v>
                       </c:pt>
@@ -3009,6 +3112,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>3.94</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>3.92</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3020,7 +3126,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2037064336"/>
+        <c:axId val="1635062672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3063,7 +3169,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037067600"/>
+        <c:crossAx val="1635051792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3071,7 +3177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2037067600"/>
+        <c:axId val="1635051792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3122,7 +3228,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037064336"/>
+        <c:crossAx val="1635062672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3297,13 +3403,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3334,6 +3440,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3365,6 +3474,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3376,14 +3488,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$W$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.1087627397260274</c:v>
                 </c:pt>
@@ -3413,6 +3525,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.0921591780821918</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.1998556164383563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3462,13 +3577,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3499,6 +3614,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>24/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>27/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3530,6 +3648,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3541,14 +3662,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$W$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.10556383561643835</c:v>
                 </c:pt>
@@ -3578,6 +3699,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.0601701369863015</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.1646676712328767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3594,8 +3718,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-155265024"/>
-        <c:axId val="-155266112"/>
+        <c:axId val="1635063216"/>
+        <c:axId val="1635053968"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3648,15 +3772,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3687,6 +3811,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3718,6 +3845,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3729,16 +3859,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$W$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2614.1</c:v>
                       </c:pt>
@@ -3768,6 +3898,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2623.9</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2626.64</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3825,15 +3958,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$W$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3864,6 +3997,9 @@
                         </c:pt>
                         <c:pt idx="9">
                           <c:v>24/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>27/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3895,6 +4031,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3906,16 +4045,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$W$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2629.97</c:v>
                       </c:pt>
@@ -3945,6 +4084,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2639.72</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2642.47</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3956,7 +4098,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-155265024"/>
+        <c:axId val="1635063216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,7 +4141,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-155266112"/>
+        <c:crossAx val="1635053968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4007,7 +4149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-155266112"/>
+        <c:axId val="1635053968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4058,7 +4200,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-155265024"/>
+        <c:crossAx val="1635063216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6457,6 +6599,7 @@
       <sheetName val="220519"/>
       <sheetName val="230519"/>
       <sheetName val="240519"/>
+      <sheetName val="270519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6495,6 +6638,7 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6521,6 +6665,7 @@
       <sheetName val="220519"/>
       <sheetName val="230519"/>
       <sheetName val="240519"/>
+      <sheetName val="270519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6554,18 +6699,19 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18">
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6944,8 +7090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6973,6 +7119,8 @@
     <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7043,8 +7191,12 @@
       <c r="W1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
+      <c r="X1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="Z1" s="20"/>
       <c r="AA1" s="20"/>
       <c r="AB1" s="20"/>
@@ -7119,11 +7271,15 @@
       <c r="V2" s="15">
         <v>43609</v>
       </c>
-      <c r="W2" s="16">
+      <c r="W2" s="17">
         <v>43609</v>
       </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="X2" s="15">
+        <v>43612</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>43612</v>
+      </c>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
       <c r="AB2" s="20"/>
@@ -7202,11 +7358,15 @@
       <c r="V3" s="36">
         <v>4.0599999999999996</v>
       </c>
-      <c r="W3" s="37">
+      <c r="W3" s="41">
         <v>2623.9</v>
       </c>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
+      <c r="X3" s="36">
+        <v>4.04</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>2626.64</v>
+      </c>
       <c r="Z3" s="20"/>
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
@@ -7285,8 +7445,14 @@
       <c r="V4" s="30">
         <v>3.94</v>
       </c>
-      <c r="W4" s="26">
+      <c r="W4" s="25">
         <v>2639.72</v>
+      </c>
+      <c r="X4" s="30">
+        <v>3.92</v>
+      </c>
+      <c r="Y4" s="26">
+        <v>2642.47</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -7380,6 +7546,14 @@
         <f t="shared" ref="W5:W6" si="15">(((V3/365)*$B$6)/100)+U5</f>
         <v>1.0921591780821918</v>
       </c>
+      <c r="X5" s="38">
+        <f t="shared" ref="X5" si="16">$B$5/Y3</f>
+        <v>0.37080982913114896</v>
+      </c>
+      <c r="Y5" s="39">
+        <f>(((X3/365)*$B$6)/100)+W5</f>
+        <v>1.1998556164383563</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -7408,7 +7582,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ref="H6" si="16">$B$6/I4</f>
+        <f t="shared" ref="H6" si="17">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="31">
@@ -7416,7 +7590,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6" si="17">$B$6/K4</f>
+        <f t="shared" ref="J6" si="18">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="31">
@@ -7424,7 +7598,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ref="L6" si="18">$B$6/M4</f>
+        <f t="shared" ref="L6" si="19">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="31">
@@ -7432,7 +7606,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6" si="19">$B$6/O4</f>
+        <f t="shared" ref="N6" si="20">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="31">
@@ -7440,7 +7614,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" ref="P6" si="20">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="21">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="31">
@@ -7448,7 +7622,7 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" ref="R6" si="21">$B$6/S4</f>
+        <f t="shared" ref="R6" si="22">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="31">
@@ -7456,7 +7630,7 @@
         <v>0.84824273972602748</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" ref="T6" si="22">$B$6/U4</f>
+        <f t="shared" ref="T6" si="23">$B$6/U4</f>
         <v>0.37005625007131093</v>
       </c>
       <c r="U6" s="31">
@@ -7464,15 +7638,21 @@
         <v>0.95513945205479467</v>
       </c>
       <c r="V6" s="29">
-        <f t="shared" ref="V6" si="23">$B$6/W4</f>
+        <f t="shared" ref="V6" si="24">$B$6/W4</f>
         <v>0.36859969996817848</v>
       </c>
       <c r="W6" s="31">
         <f t="shared" si="15"/>
         <v>1.0601701369863015</v>
       </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
+      <c r="X6" s="29">
+        <f t="shared" ref="X6" si="25">$B$6/Y4</f>
+        <v>0.36821610084504275</v>
+      </c>
+      <c r="Y6" s="31">
+        <f t="shared" ref="Y5:Y6" si="26">(((X4/365)*$B$6)/100)+W6</f>
+        <v>1.1646676712328767</v>
+      </c>
       <c r="Z6" s="22"/>
       <c r="AA6" s="22"/>
       <c r="AB6" s="22"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 28/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -487,13 +487,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -527,6 +527,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -561,6 +564,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -572,14 +578,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3)</c:f>
+              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>4.08</c:v>
                 </c:pt>
@@ -612,6 +618,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,13 +670,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -701,6 +710,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -735,6 +747,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -746,14 +761,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4)</c:f>
+              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.96</c:v>
                 </c:pt>
@@ -786,6 +801,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.92</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>3.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -802,8 +820,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1635059952"/>
-        <c:axId val="1635061584"/>
+        <c:axId val="105664320"/>
+        <c:axId val="105665408"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -856,15 +874,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -898,6 +916,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -932,6 +953,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -943,16 +967,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.37258862690373018</c:v>
                       </c:pt>
@@ -985,6 +1009,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
                         <c:v>0.37080982913114896</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="0.00">
+                        <c:v>0.37016719732024972</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1042,15 +1069,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1084,6 +1111,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1118,6 +1148,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1129,16 +1162,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.36996619733304947</c:v>
                       </c:pt>
@@ -1171,6 +1204,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
                         <c:v>0.36821610084504275</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="0.00">
+                        <c:v>0.36757900304112123</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1182,7 +1218,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1635059952"/>
+        <c:axId val="105664320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,7 +1261,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635061584"/>
+        <c:crossAx val="105665408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1233,7 +1269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1635061584"/>
+        <c:axId val="105665408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1320,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635059952"/>
+        <c:crossAx val="105664320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,13 +1495,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1499,6 +1535,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1533,6 +1572,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1544,14 +1586,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3)</c:f>
+              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2614.1</c:v>
                 </c:pt>
@@ -1584,6 +1626,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2626.64</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2631.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,13 +1678,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1673,6 +1718,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1707,6 +1755,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1718,14 +1769,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2629.97</c:v>
                 </c:pt>
@@ -1758,6 +1809,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2642.47</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2647.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1774,8 +1828,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1635062128"/>
-        <c:axId val="1635053424"/>
+        <c:axId val="105664864"/>
+        <c:axId val="105665952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1828,15 +1882,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1870,6 +1924,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1904,6 +1961,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1915,16 +1975,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.1087627397260274</c:v>
                       </c:pt>
@@ -1957,6 +2017,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.1998556164383563</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.3067523287671234</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2014,15 +2077,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2056,6 +2119,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2090,6 +2156,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2101,16 +2170,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.10556383561643835</c:v>
                       </c:pt>
@@ -2143,6 +2212,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.1646676712328767</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.2683654794520549</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2154,7 +2226,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1635062128"/>
+        <c:axId val="105664864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,7 +2269,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635053424"/>
+        <c:crossAx val="105665952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2205,7 +2277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1635053424"/>
+        <c:axId val="105665952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2328,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635062128"/>
+        <c:crossAx val="105664864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2431,13 +2503,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2471,6 +2543,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2505,6 +2580,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2516,14 +2594,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5)</c:f>
+              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.37258862690373018</c:v>
                 </c:pt>
@@ -2556,6 +2634,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
                   <c:v>0.37080982913114896</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.37016719732024972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2605,13 +2686,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2645,6 +2726,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2679,6 +2763,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2690,14 +2777,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.36996619733304947</c:v>
                 </c:pt>
@@ -2730,6 +2817,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
                   <c:v>0.36821610084504275</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.36757900304112123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2746,8 +2836,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1635062672"/>
-        <c:axId val="1635051792"/>
+        <c:axId val="105666496"/>
+        <c:axId val="105667584"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2800,15 +2890,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2842,6 +2932,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2876,6 +2969,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2887,16 +2983,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>4.08</c:v>
                       </c:pt>
@@ -2929,6 +3025,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.04</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.01</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2986,15 +3085,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3028,6 +3127,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3062,6 +3164,9 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3073,16 +3178,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>3.96</c:v>
                       </c:pt>
@@ -3115,6 +3220,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.92</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>3.89</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3126,7 +3234,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1635062672"/>
+        <c:axId val="105666496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3169,7 +3277,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635051792"/>
+        <c:crossAx val="105667584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3177,7 +3285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1635051792"/>
+        <c:axId val="105667584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3228,7 +3336,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635062672"/>
+        <c:crossAx val="105666496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3403,13 +3511,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3443,6 +3551,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3477,6 +3588,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3488,14 +3602,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$Y$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.1087627397260274</c:v>
                 </c:pt>
@@ -3528,6 +3642,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.1998556164383563</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.3067523287671234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3577,13 +3694,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3617,6 +3734,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>27/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>28/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3651,6 +3771,9 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3662,14 +3785,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$Y$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.10556383561643835</c:v>
                 </c:pt>
@@ -3702,6 +3825,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.1646676712328767</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.2683654794520549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3718,8 +3844,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1635063216"/>
-        <c:axId val="1635053968"/>
+        <c:axId val="105663232"/>
+        <c:axId val="105667040"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3772,15 +3898,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3814,6 +3940,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3848,6 +3977,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3859,16 +3991,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$Y$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2614.1</c:v>
                       </c:pt>
@@ -3901,6 +4033,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2626.64</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2631.2</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3958,15 +4093,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$Y$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -4000,6 +4135,9 @@
                         </c:pt>
                         <c:pt idx="10">
                           <c:v>27/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>28/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -4034,6 +4172,9 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4045,16 +4186,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$Y$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2629.97</c:v>
                       </c:pt>
@@ -4087,6 +4228,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2642.47</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2647.05</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4098,7 +4242,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1635063216"/>
+        <c:axId val="105663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4141,7 +4285,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635053968"/>
+        <c:crossAx val="105667040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4149,7 +4293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1635053968"/>
+        <c:axId val="105667040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4200,7 +4344,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635063216"/>
+        <c:crossAx val="105663232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6600,6 +6744,7 @@
       <sheetName val="230519"/>
       <sheetName val="240519"/>
       <sheetName val="270519"/>
+      <sheetName val="280519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6639,6 +6784,7 @@
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6666,6 +6812,7 @@
       <sheetName val="230519"/>
       <sheetName val="240519"/>
       <sheetName val="270519"/>
+      <sheetName val="280519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6700,18 +6847,19 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7090,8 +7238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7121,6 +7269,8 @@
     <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7197,8 +7347,12 @@
       <c r="Y1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
+      <c r="Z1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="AB1" s="20"/>
       <c r="AC1" s="20"/>
       <c r="AD1" s="20"/>
@@ -7280,8 +7434,12 @@
       <c r="Y2" s="16">
         <v>43612</v>
       </c>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
+      <c r="Z2" s="15">
+        <v>43613</v>
+      </c>
+      <c r="AA2" s="16">
+        <v>43613</v>
+      </c>
       <c r="AB2" s="20"/>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
@@ -7364,11 +7522,15 @@
       <c r="X3" s="36">
         <v>4.04</v>
       </c>
-      <c r="Y3" s="37">
+      <c r="Y3" s="41">
         <v>2626.64</v>
       </c>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
+      <c r="Z3" s="36">
+        <v>4.01</v>
+      </c>
+      <c r="AA3" s="37">
+        <v>2631.2</v>
+      </c>
       <c r="AB3" s="20"/>
       <c r="AC3" s="20"/>
       <c r="AD3" s="20"/>
@@ -7451,8 +7613,14 @@
       <c r="X4" s="30">
         <v>3.92</v>
       </c>
-      <c r="Y4" s="26">
+      <c r="Y4" s="25">
         <v>2642.47</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>3.89</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>2647.05</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -7554,6 +7722,14 @@
         <f>(((X3/365)*$B$6)/100)+W5</f>
         <v>1.1998556164383563</v>
       </c>
+      <c r="Z5" s="38">
+        <f t="shared" ref="Z5" si="17">$B$5/AA3</f>
+        <v>0.37016719732024972</v>
+      </c>
+      <c r="AA5" s="39">
+        <f>(((Z3/365)*$B$6)/100)+Y5</f>
+        <v>1.3067523287671234</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -7582,7 +7758,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ref="H6" si="17">$B$6/I4</f>
+        <f t="shared" ref="H6" si="18">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="31">
@@ -7590,7 +7766,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6" si="18">$B$6/K4</f>
+        <f t="shared" ref="J6" si="19">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="31">
@@ -7598,7 +7774,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ref="L6" si="19">$B$6/M4</f>
+        <f t="shared" ref="L6" si="20">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="31">
@@ -7606,7 +7782,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6" si="20">$B$6/O4</f>
+        <f t="shared" ref="N6" si="21">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="31">
@@ -7614,7 +7790,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" ref="P6" si="21">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="22">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="31">
@@ -7622,7 +7798,7 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" ref="R6" si="22">$B$6/S4</f>
+        <f t="shared" ref="R6" si="23">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="31">
@@ -7630,7 +7806,7 @@
         <v>0.84824273972602748</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" ref="T6" si="23">$B$6/U4</f>
+        <f t="shared" ref="T6" si="24">$B$6/U4</f>
         <v>0.37005625007131093</v>
       </c>
       <c r="U6" s="31">
@@ -7638,7 +7814,7 @@
         <v>0.95513945205479467</v>
       </c>
       <c r="V6" s="29">
-        <f t="shared" ref="V6" si="24">$B$6/W4</f>
+        <f t="shared" ref="V6" si="25">$B$6/W4</f>
         <v>0.36859969996817848</v>
       </c>
       <c r="W6" s="31">
@@ -7646,15 +7822,21 @@
         <v>1.0601701369863015</v>
       </c>
       <c r="X6" s="29">
-        <f t="shared" ref="X6" si="25">$B$6/Y4</f>
+        <f t="shared" ref="X6" si="26">$B$6/Y4</f>
         <v>0.36821610084504275</v>
       </c>
       <c r="Y6" s="31">
-        <f t="shared" ref="Y5:Y6" si="26">(((X4/365)*$B$6)/100)+W6</f>
+        <f t="shared" ref="Y6" si="27">(((X4/365)*$B$6)/100)+W6</f>
         <v>1.1646676712328767</v>
       </c>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
+      <c r="Z6" s="29">
+        <f t="shared" ref="Z6" si="28">$B$6/AA4</f>
+        <v>0.36757900304112123</v>
+      </c>
+      <c r="AA6" s="31">
+        <f t="shared" ref="AA6" si="29">(((Z4/365)*$B$6)/100)+Y6</f>
+        <v>1.2683654794520549</v>
+      </c>
       <c r="AB6" s="22"/>
       <c r="AC6" s="22"/>
       <c r="AD6" s="22"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 29/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>Tesouro IPCA+ 2024</t>
+  </si>
+  <si>
+    <t>Tesouro IPCA+</t>
+  </si>
+  <si>
+    <t>Títulos</t>
+  </si>
+  <si>
+    <t>Últ. 30 dias</t>
+  </si>
+  <si>
+    <t>No ano</t>
+  </si>
+  <si>
+    <t>12 meses</t>
+  </si>
+  <si>
+    <t>Compra</t>
+  </si>
+  <si>
+    <t>Venda</t>
+  </si>
+  <si>
+    <t>Mês Anterior</t>
   </si>
 </sst>
 </file>
@@ -267,7 +291,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,6 +398,7 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -408,7 +433,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -820,8 +844,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105664320"/>
-        <c:axId val="105665408"/>
+        <c:axId val="1150685920"/>
+        <c:axId val="1150689184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1025,7 +1049,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -1218,7 +1242,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105664320"/>
+        <c:axId val="1150685920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,7 +1285,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105665408"/>
+        <c:crossAx val="1150689184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1269,7 +1293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105665408"/>
+        <c:axId val="1150689184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1344,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105664320"/>
+        <c:crossAx val="1150685920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1334,7 +1358,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1416,7 +1439,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1828,8 +1850,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105664864"/>
-        <c:axId val="105665952"/>
+        <c:axId val="1150675584"/>
+        <c:axId val="1150676128"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2033,7 +2055,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -2226,7 +2248,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105664864"/>
+        <c:axId val="1150675584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,7 +2291,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105665952"/>
+        <c:crossAx val="1150676128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2277,7 +2299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105665952"/>
+        <c:axId val="1150676128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,7 +2350,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105664864"/>
+        <c:crossAx val="1150675584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2342,7 +2364,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2836,8 +2857,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105666496"/>
-        <c:axId val="105667584"/>
+        <c:axId val="1150678304"/>
+        <c:axId val="1150686464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3041,7 +3062,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -3234,7 +3255,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105666496"/>
+        <c:axId val="1150678304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3277,7 +3298,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105667584"/>
+        <c:crossAx val="1150686464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3285,7 +3306,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105667584"/>
+        <c:axId val="1150686464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3357,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105666496"/>
+        <c:crossAx val="1150678304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3844,8 +3865,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105663232"/>
-        <c:axId val="105667040"/>
+        <c:axId val="1150676672"/>
+        <c:axId val="1150683200"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4049,7 +4070,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -4242,7 +4263,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105663232"/>
+        <c:axId val="1150676672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4285,7 +4306,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105667040"/>
+        <c:crossAx val="1150683200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4293,7 +4314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105667040"/>
+        <c:axId val="1150683200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4344,7 +4365,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105663232"/>
+        <c:crossAx val="1150676672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6745,6 +6766,7 @@
       <sheetName val="240519"/>
       <sheetName val="270519"/>
       <sheetName val="280519"/>
+      <sheetName val="290519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6785,6 +6807,7 @@
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6813,6 +6836,7 @@
       <sheetName val="240519"/>
       <sheetName val="270519"/>
       <sheetName val="280519"/>
+      <sheetName val="290519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6848,18 +6872,19 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
-      <sheetData sheetId="20">
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
       <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7152,10 +7177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7163,7 +7188,7 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
@@ -7227,6 +7252,84 @@
       <c r="H2" s="9">
         <f>'[2]TESOURO IPCA'!$R$5</f>
         <v>2614.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="46">
+        <v>45519</v>
+      </c>
+      <c r="C5">
+        <v>1.49</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>6.57</v>
+      </c>
+      <c r="F5">
+        <v>17.57</v>
+      </c>
+      <c r="G5">
+        <v>3.89</v>
+      </c>
+      <c r="H5">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <f>((C2*C5)/100)+C2</f>
+        <v>987.49770000000001</v>
+      </c>
+      <c r="D7" s="9">
+        <f>((C2*D5)/100)+C2</f>
+        <v>977.86500000000001</v>
+      </c>
+      <c r="E7" s="9">
+        <f>((C2*E5)/100)+C2</f>
+        <v>1036.9260999999999</v>
+      </c>
+      <c r="F7" s="9">
+        <f>((C2*F5)/100)+C2</f>
+        <v>1143.9560999999999</v>
+      </c>
+      <c r="G7">
+        <f>E2-G5</f>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="H7">
+        <f>G2-H5</f>
+        <v>0.54999999999999982</v>
       </c>
     </row>
   </sheetData>
@@ -7238,8 +7341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7271,6 +7374,8 @@
     <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7353,8 +7458,12 @@
       <c r="AA1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
+      <c r="AB1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="AD1" s="20"/>
       <c r="AE1" s="20"/>
       <c r="AF1" s="20"/>
@@ -7440,8 +7549,12 @@
       <c r="AA2" s="16">
         <v>43613</v>
       </c>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
+      <c r="AB2" s="15">
+        <v>43614</v>
+      </c>
+      <c r="AC2" s="16">
+        <v>43614</v>
+      </c>
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
       <c r="AF2" s="20"/>
@@ -7528,11 +7641,15 @@
       <c r="Z3" s="36">
         <v>4.01</v>
       </c>
-      <c r="AA3" s="37">
+      <c r="AA3" s="41">
         <v>2631.2</v>
       </c>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
+      <c r="AB3" s="36">
+        <v>3.83</v>
+      </c>
+      <c r="AC3" s="37">
+        <v>2655.62</v>
+      </c>
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
       <c r="AF3" s="20"/>
@@ -7619,8 +7736,14 @@
       <c r="Z4" s="30">
         <v>3.89</v>
       </c>
-      <c r="AA4" s="26">
+      <c r="AA4" s="25">
         <v>2647.05</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>3.71</v>
+      </c>
+      <c r="AC4" s="26">
+        <v>2671.63</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -7730,6 +7853,14 @@
         <f>(((Z3/365)*$B$6)/100)+Y5</f>
         <v>1.3067523287671234</v>
       </c>
+      <c r="AB5" s="38">
+        <f t="shared" ref="AB5" si="18">$B$5/AC3</f>
+        <v>0.3667632905268981</v>
+      </c>
+      <c r="AC5" s="39">
+        <f>(((AB3/365)*$B$6)/100)+AA5</f>
+        <v>1.408850684931507</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -7758,7 +7889,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ref="H6" si="18">$B$6/I4</f>
+        <f t="shared" ref="H6" si="19">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="31">
@@ -7766,7 +7897,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6" si="19">$B$6/K4</f>
+        <f t="shared" ref="J6" si="20">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="31">
@@ -7774,7 +7905,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ref="L6" si="20">$B$6/M4</f>
+        <f t="shared" ref="L6" si="21">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="31">
@@ -7782,7 +7913,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6" si="21">$B$6/O4</f>
+        <f t="shared" ref="N6" si="22">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="31">
@@ -7790,7 +7921,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" ref="P6" si="22">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="23">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="31">
@@ -7798,7 +7929,7 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" ref="R6" si="23">$B$6/S4</f>
+        <f t="shared" ref="R6" si="24">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="31">
@@ -7806,7 +7937,7 @@
         <v>0.84824273972602748</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" ref="T6" si="24">$B$6/U4</f>
+        <f t="shared" ref="T6" si="25">$B$6/U4</f>
         <v>0.37005625007131093</v>
       </c>
       <c r="U6" s="31">
@@ -7814,7 +7945,7 @@
         <v>0.95513945205479467</v>
       </c>
       <c r="V6" s="29">
-        <f t="shared" ref="V6" si="25">$B$6/W4</f>
+        <f t="shared" ref="V6" si="26">$B$6/W4</f>
         <v>0.36859969996817848</v>
       </c>
       <c r="W6" s="31">
@@ -7822,23 +7953,29 @@
         <v>1.0601701369863015</v>
       </c>
       <c r="X6" s="29">
-        <f t="shared" ref="X6" si="26">$B$6/Y4</f>
+        <f t="shared" ref="X6" si="27">$B$6/Y4</f>
         <v>0.36821610084504275</v>
       </c>
       <c r="Y6" s="31">
-        <f t="shared" ref="Y6" si="27">(((X4/365)*$B$6)/100)+W6</f>
+        <f t="shared" ref="Y6" si="28">(((X4/365)*$B$6)/100)+W6</f>
         <v>1.1646676712328767</v>
       </c>
       <c r="Z6" s="29">
-        <f t="shared" ref="Z6" si="28">$B$6/AA4</f>
+        <f t="shared" ref="Z6" si="29">$B$6/AA4</f>
         <v>0.36757900304112123</v>
       </c>
       <c r="AA6" s="31">
-        <f t="shared" ref="AA6" si="29">(((Z4/365)*$B$6)/100)+Y6</f>
+        <f t="shared" ref="AA6" si="30">(((Z4/365)*$B$6)/100)+Y6</f>
         <v>1.2683654794520549</v>
       </c>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
+      <c r="AB6" s="29">
+        <f t="shared" ref="AB6" si="31">$B$6/AC4</f>
+        <v>0.36419713807675463</v>
+      </c>
+      <c r="AC6" s="31">
+        <f t="shared" ref="AC6" si="32">(((AB4/365)*$B$6)/100)+AA6</f>
+        <v>1.3672649315068495</v>
+      </c>
       <c r="AD6" s="22"/>
       <c r="AE6" s="22"/>
       <c r="AF6" s="22"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 30/05 - criacao acomanhamento mes 06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -844,8 +844,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1150685920"/>
-        <c:axId val="1150689184"/>
+        <c:axId val="-1428113376"/>
+        <c:axId val="-1428116640"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1242,7 +1242,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1150685920"/>
+        <c:axId val="-1428113376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1285,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150689184"/>
+        <c:crossAx val="-1428116640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1293,7 +1293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150689184"/>
+        <c:axId val="-1428116640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1344,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150685920"/>
+        <c:crossAx val="-1428113376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1850,8 +1850,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1150675584"/>
-        <c:axId val="1150676128"/>
+        <c:axId val="-1428110656"/>
+        <c:axId val="-1428116096"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2248,7 +2248,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1150675584"/>
+        <c:axId val="-1428110656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2291,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150676128"/>
+        <c:crossAx val="-1428116096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2299,7 +2299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150676128"/>
+        <c:axId val="-1428116096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2350,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150675584"/>
+        <c:crossAx val="-1428110656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2445,7 +2445,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2857,8 +2856,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1150678304"/>
-        <c:axId val="1150686464"/>
+        <c:axId val="-1428115008"/>
+        <c:axId val="-1428109568"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3255,7 +3254,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1150678304"/>
+        <c:axId val="-1428115008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3298,7 +3297,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150686464"/>
+        <c:crossAx val="-1428109568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3306,7 +3305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150686464"/>
+        <c:axId val="-1428109568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3357,7 +3356,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150678304"/>
+        <c:crossAx val="-1428115008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3371,7 +3370,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3453,7 +3451,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3865,8 +3862,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1150676672"/>
-        <c:axId val="1150683200"/>
+        <c:axId val="-1428109024"/>
+        <c:axId val="-1428118272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4263,7 +4260,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1150676672"/>
+        <c:axId val="-1428109024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4306,7 +4303,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150683200"/>
+        <c:crossAx val="-1428118272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4314,7 +4311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150683200"/>
+        <c:axId val="-1428118272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4365,7 +4362,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150676672"/>
+        <c:crossAx val="-1428109024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4379,7 +4376,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6767,6 +6763,7 @@
       <sheetName val="270519"/>
       <sheetName val="280519"/>
       <sheetName val="290519"/>
+      <sheetName val="300519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6808,6 +6805,7 @@
       <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6837,6 +6835,7 @@
       <sheetName val="270519"/>
       <sheetName val="280519"/>
       <sheetName val="290519"/>
+      <sheetName val="300519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6873,18 +6872,19 @@
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
-      <sheetData sheetId="21">
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="22"/>
       <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7341,8 +7341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7376,6 +7376,8 @@
     <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7464,8 +7466,12 @@
       <c r="AC1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
+      <c r="AD1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
       <c r="AH1" s="20"/>
@@ -7555,8 +7561,12 @@
       <c r="AC2" s="16">
         <v>43614</v>
       </c>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
+      <c r="AD2" s="15">
+        <v>43615</v>
+      </c>
+      <c r="AE2" s="16">
+        <v>43615</v>
+      </c>
       <c r="AF2" s="20"/>
       <c r="AG2" s="20"/>
       <c r="AH2" s="20"/>
@@ -7647,11 +7657,15 @@
       <c r="AB3" s="36">
         <v>3.83</v>
       </c>
-      <c r="AC3" s="37">
+      <c r="AC3" s="41">
         <v>2655.62</v>
       </c>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
+      <c r="AD3" s="36">
+        <v>3.83</v>
+      </c>
+      <c r="AE3" s="37">
+        <v>2656.22</v>
+      </c>
       <c r="AF3" s="20"/>
       <c r="AG3" s="20"/>
       <c r="AH3" s="20"/>
@@ -7742,8 +7756,14 @@
       <c r="AB4" s="30">
         <v>3.71</v>
       </c>
-      <c r="AC4" s="26">
+      <c r="AC4" s="25">
         <v>2671.63</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>3.71</v>
+      </c>
+      <c r="AE4" s="26">
+        <v>2672.22</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -7861,6 +7881,14 @@
         <f>(((AB3/365)*$B$6)/100)+AA5</f>
         <v>1.408850684931507</v>
       </c>
+      <c r="AD5" s="38">
+        <f t="shared" ref="AD5" si="19">$B$5/AE3</f>
+        <v>0.36668044423618568</v>
+      </c>
+      <c r="AE5" s="39">
+        <f>(((AD3/365)*$B$6)/100)+AC5</f>
+        <v>1.5109490410958906</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -7889,7 +7917,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ref="H6" si="19">$B$6/I4</f>
+        <f t="shared" ref="H6" si="20">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="31">
@@ -7897,7 +7925,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6" si="20">$B$6/K4</f>
+        <f t="shared" ref="J6" si="21">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="31">
@@ -7905,7 +7933,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ref="L6" si="21">$B$6/M4</f>
+        <f t="shared" ref="L6" si="22">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="31">
@@ -7913,7 +7941,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6" si="22">$B$6/O4</f>
+        <f t="shared" ref="N6" si="23">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="31">
@@ -7921,7 +7949,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" ref="P6" si="23">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="24">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="31">
@@ -7929,7 +7957,7 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" ref="R6" si="24">$B$6/S4</f>
+        <f t="shared" ref="R6" si="25">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="31">
@@ -7937,7 +7965,7 @@
         <v>0.84824273972602748</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" ref="T6" si="25">$B$6/U4</f>
+        <f t="shared" ref="T6" si="26">$B$6/U4</f>
         <v>0.37005625007131093</v>
       </c>
       <c r="U6" s="31">
@@ -7945,7 +7973,7 @@
         <v>0.95513945205479467</v>
       </c>
       <c r="V6" s="29">
-        <f t="shared" ref="V6" si="26">$B$6/W4</f>
+        <f t="shared" ref="V6" si="27">$B$6/W4</f>
         <v>0.36859969996817848</v>
       </c>
       <c r="W6" s="31">
@@ -7953,31 +7981,37 @@
         <v>1.0601701369863015</v>
       </c>
       <c r="X6" s="29">
-        <f t="shared" ref="X6" si="27">$B$6/Y4</f>
+        <f t="shared" ref="X6" si="28">$B$6/Y4</f>
         <v>0.36821610084504275</v>
       </c>
       <c r="Y6" s="31">
-        <f t="shared" ref="Y6" si="28">(((X4/365)*$B$6)/100)+W6</f>
+        <f t="shared" ref="Y6" si="29">(((X4/365)*$B$6)/100)+W6</f>
         <v>1.1646676712328767</v>
       </c>
       <c r="Z6" s="29">
-        <f t="shared" ref="Z6" si="29">$B$6/AA4</f>
+        <f t="shared" ref="Z6" si="30">$B$6/AA4</f>
         <v>0.36757900304112123</v>
       </c>
       <c r="AA6" s="31">
-        <f t="shared" ref="AA6" si="30">(((Z4/365)*$B$6)/100)+Y6</f>
+        <f t="shared" ref="AA6" si="31">(((Z4/365)*$B$6)/100)+Y6</f>
         <v>1.2683654794520549</v>
       </c>
       <c r="AB6" s="29">
-        <f t="shared" ref="AB6" si="31">$B$6/AC4</f>
+        <f t="shared" ref="AB6" si="32">$B$6/AC4</f>
         <v>0.36419713807675463</v>
       </c>
       <c r="AC6" s="31">
-        <f t="shared" ref="AC6" si="32">(((AB4/365)*$B$6)/100)+AA6</f>
+        <f t="shared" ref="AC6" si="33">(((AB4/365)*$B$6)/100)+AA6</f>
         <v>1.3672649315068495</v>
       </c>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
+      <c r="AD6" s="29">
+        <f t="shared" ref="AD6" si="34">$B$6/AE4</f>
+        <v>0.36411672691619706</v>
+      </c>
+      <c r="AE6" s="31">
+        <f t="shared" ref="AE6" si="35">(((AD4/365)*$B$6)/100)+AC6</f>
+        <v>1.466164383561644</v>
+      </c>
       <c r="AF6" s="22"/>
       <c r="AG6" s="22"/>
       <c r="AH6" s="22"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 31/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>TÍTULO COMPRADO</t>
   </si>
@@ -291,7 +291,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,6 +399,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -433,6 +435,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -511,13 +514,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -554,6 +557,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -591,6 +603,15 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -602,14 +623,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$AG$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3)</c:f>
+              <c:f>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3,GRAFICO!$AB$3,GRAFICO!$AD$3,GRAFICO!$AF$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>4.08</c:v>
                 </c:pt>
@@ -645,6 +666,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
                   <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>3.83</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>3.83</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>3.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,13 +724,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -737,6 +767,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -774,6 +813,15 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -785,14 +833,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4)</c:f>
+              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.96</c:v>
                 </c:pt>
@@ -828,6 +876,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
                   <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,8 +901,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1428113376"/>
-        <c:axId val="-1428116640"/>
+        <c:axId val="-612754720"/>
+        <c:axId val="-612761792"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -898,15 +955,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -943,6 +1000,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -980,6 +1046,15 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -991,16 +1066,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.37258862690373018</c:v>
                       </c:pt>
@@ -1036,6 +1111,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
                         <c:v>0.37016719732024972</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="0.00">
+                        <c:v>0.3667632905268981</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="0.00">
+                        <c:v>0.36668044423618568</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="0.00">
+                        <c:v>0.36635770100695153</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1049,7 +1133,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -1093,15 +1177,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1138,6 +1222,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1175,6 +1268,15 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1186,16 +1288,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="0.00">
                         <c:v>0.36996619733304947</c:v>
                       </c:pt>
@@ -1231,6 +1333,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
                         <c:v>0.36757900304112123</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="0.00">
+                        <c:v>0.36419713807675463</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="0.00">
+                        <c:v>0.36411672691619706</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="0.00">
+                        <c:v>0.36379679724217351</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1242,7 +1353,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1428113376"/>
+        <c:axId val="-612754720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1396,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428116640"/>
+        <c:crossAx val="-612761792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1293,7 +1404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1428116640"/>
+        <c:axId val="-612761792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1455,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428113376"/>
+        <c:crossAx val="-612754720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,6 +1469,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1439,6 +1551,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1517,13 +1630,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1560,6 +1673,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1597,6 +1719,15 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1608,14 +1739,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$3:$AG$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3)</c:f>
+              <c:f>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3,GRAFICO!$AC$3,GRAFICO!$AE$3,GRAFICO!$AG$3)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2614.1</c:v>
                 </c:pt>
@@ -1651,6 +1782,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2631.2</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2655.62</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2656.22</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2658.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1700,13 +1840,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -1743,6 +1883,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1780,6 +1929,15 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1791,14 +1949,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2629.97</c:v>
                 </c:pt>
@@ -1834,6 +1992,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2647.05</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2671.63</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2672.22</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>2674.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1850,8 +2017,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1428110656"/>
-        <c:axId val="-1428116096"/>
+        <c:axId val="-612762880"/>
+        <c:axId val="-612757984"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1904,15 +2071,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -1949,6 +2116,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1986,6 +2162,15 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1997,16 +2182,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.1087627397260274</c:v>
                       </c:pt>
@@ -2042,6 +2227,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.3067523287671234</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.408850684931507</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.5109490410958906</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.6127808219178084</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2055,7 +2249,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -2099,15 +2293,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2144,6 +2338,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2181,6 +2384,15 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -2192,16 +2404,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>0.10556383561643835</c:v>
                       </c:pt>
@@ -2237,6 +2449,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                         <c:v>1.2683654794520549</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.3672649315068495</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.466164383561644</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                        <c:v>1.5647972602739728</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2248,7 +2469,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1428110656"/>
+        <c:axId val="-612762880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2512,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428116096"/>
+        <c:crossAx val="-612757984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2299,7 +2520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1428116096"/>
+        <c:axId val="-612757984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2571,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428110656"/>
+        <c:crossAx val="-612762880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2364,6 +2585,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2445,6 +2667,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2523,13 +2746,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2566,6 +2789,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2603,6 +2835,15 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2614,14 +2855,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5)</c:f>
+              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.37258862690373018</c:v>
                 </c:pt>
@@ -2657,6 +2898,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
                   <c:v>0.37016719732024972</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.3667632905268981</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.36668044423618568</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>0.36635770100695153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2706,13 +2956,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c:f>
+              <c:f>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -2749,6 +2999,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2786,6 +3045,15 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2797,14 +3065,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.36996619733304947</c:v>
                 </c:pt>
@@ -2840,6 +3108,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
                   <c:v>0.36757900304112123</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.36419713807675463</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.36411672691619706</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>0.36379679724217351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2856,8 +3133,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1428115008"/>
-        <c:axId val="-1428109568"/>
+        <c:axId val="-612759072"/>
+        <c:axId val="-612765600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2910,15 +3187,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -2955,6 +3232,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -2992,6 +3278,15 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3003,16 +3298,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$AG$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$3,GRAFICO!$F$3,GRAFICO!$H$3,GRAFICO!$J$3,GRAFICO!$L$3,GRAFICO!$N$3,GRAFICO!$P$3,GRAFICO!$R$3,GRAFICO!$T$3,GRAFICO!$V$3,GRAFICO!$X$3,GRAFICO!$Z$3,GRAFICO!$AB$3,GRAFICO!$AD$3,GRAFICO!$AF$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>4.08</c:v>
                       </c:pt>
@@ -3048,6 +3343,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="General">
                         <c:v>4.01</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>3.83</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>3.83</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="General">
+                        <c:v>3.82</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3061,7 +3365,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -3105,15 +3409,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$1:$D$2,GRAFICO!$F$1:$F$2,GRAFICO!$H$1:$H$2,GRAFICO!$J$1:$J$2,GRAFICO!$L$1:$L$2,GRAFICO!$N$1:$N$2,GRAFICO!$P$1:$P$2,GRAFICO!$R$1:$R$2,GRAFICO!$T$1:$T$2,GRAFICO!$V$1:$V$2,GRAFICO!$X$1:$X$2,GRAFICO!$Z$1:$Z$2,GRAFICO!$AB$1:$AB$2,GRAFICO!$AD$1:$AD$2,GRAFICO!$AF$1:$AF$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3150,6 +3454,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3187,6 +3500,15 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3198,16 +3520,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>3.96</c:v>
                       </c:pt>
@@ -3243,6 +3565,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="General">
                         <c:v>3.89</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>3.71</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>3.71</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="General">
+                        <c:v>3.7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3254,7 +3585,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1428115008"/>
+        <c:axId val="-612759072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3297,7 +3628,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428109568"/>
+        <c:crossAx val="-612765600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3305,7 +3636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1428109568"/>
+        <c:axId val="-612765600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3356,7 +3687,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428115008"/>
+        <c:crossAx val="-612759072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3370,6 +3701,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3451,6 +3783,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3529,13 +3862,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3572,6 +3905,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3609,6 +3951,15 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3620,14 +3971,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$AA$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.1087627397260274</c:v>
                 </c:pt>
@@ -3663,6 +4014,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.3067523287671234</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.408850684931507</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.5109490410958906</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.6127808219178084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3712,13 +4072,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c:f>
+              <c:f>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>13/mai</c:v>
@@ -3755,6 +4115,15 @@
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>28/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>29/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>30/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>31/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3792,6 +4161,15 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3803,14 +4181,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AA$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.10556383561643835</c:v>
                 </c:pt>
@@ -3846,6 +4224,15 @@
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>1.2683654794520549</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.3672649315068495</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.466164383561644</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1.5647972602739728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3862,8 +4249,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1428109024"/>
-        <c:axId val="-1428118272"/>
+        <c:axId val="-612753088"/>
+        <c:axId val="-612751456"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3916,15 +4303,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -3961,6 +4348,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3998,6 +4394,15 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4009,16 +4414,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$3:$AA$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$3:$AG$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$3,GRAFICO!$G$3,GRAFICO!$I$3,GRAFICO!$K$3,GRAFICO!$M$3,GRAFICO!$O$3,GRAFICO!$Q$3,GRAFICO!$S$3,GRAFICO!$U$3,GRAFICO!$W$3,GRAFICO!$Y$3,GRAFICO!$AA$3,GRAFICO!$AC$3,GRAFICO!$AE$3,GRAFICO!$AG$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2614.1</c:v>
                       </c:pt>
@@ -4054,6 +4459,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2631.2</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2655.62</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2656.22</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2658.56</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4067,7 +4481,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -4111,15 +4525,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$1:$AA$2</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$1:$AG$2</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$1:$E$2,GRAFICO!$G$1:$G$2,GRAFICO!$I$1:$I$2,GRAFICO!$K$1:$K$2,GRAFICO!$M$1:$M$2,GRAFICO!$O$1:$O$2,GRAFICO!$Q$1:$Q$2,GRAFICO!$S$1:$S$2,GRAFICO!$U$1:$U$2,GRAFICO!$W$1:$W$2,GRAFICO!$Y$1:$Y$2,GRAFICO!$AA$1:$AA$2,GRAFICO!$AC$1:$AC$2,GRAFICO!$AE$1:$AE$2,GRAFICO!$AG$1:$AG$2)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>13/mai</c:v>
@@ -4156,6 +4570,15 @@
                         </c:pt>
                         <c:pt idx="11">
                           <c:v>28/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>29/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>30/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>31/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -4193,6 +4616,15 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4204,16 +4636,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AA$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2629.97</c:v>
                       </c:pt>
@@ -4249,6 +4681,15 @@
                       </c:pt>
                       <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>2647.05</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2671.63</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2672.22</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>2674.57</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4260,7 +4701,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1428109024"/>
+        <c:axId val="-612753088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4744,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428118272"/>
+        <c:crossAx val="-612751456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4311,7 +4752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1428118272"/>
+        <c:axId val="-612751456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,7 +4803,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428109024"/>
+        <c:crossAx val="-612753088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4376,6 +4817,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6764,6 +7206,7 @@
       <sheetName val="280519"/>
       <sheetName val="290519"/>
       <sheetName val="300519"/>
+      <sheetName val="310519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6806,6 +7249,7 @@
       <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
       <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6836,6 +7280,7 @@
       <sheetName val="280519"/>
       <sheetName val="290519"/>
       <sheetName val="300519"/>
+      <sheetName val="310519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6873,18 +7318,19 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
-      <sheetData sheetId="22">
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23">
         <row r="5">
           <cell r="R5">
             <v>2614.1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="23"/>
       <sheetData sheetId="24"/>
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7339,10 +7785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7378,9 +7824,11 @@
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34"/>
       <c r="B1" s="11" t="s">
         <v>8</v>
@@ -7472,12 +7920,15 @@
       <c r="AE1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
+      <c r="AF1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
     </row>
-    <row r="2" spans="1:35" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="14" t="s">
         <v>12</v>
@@ -7567,12 +8018,15 @@
       <c r="AE2" s="16">
         <v>43615</v>
       </c>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
+      <c r="AF2" s="15">
+        <v>43616</v>
+      </c>
+      <c r="AG2" s="16">
+        <v>43616</v>
+      </c>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
     </row>
-    <row r="3" spans="1:35" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
@@ -7663,15 +8117,18 @@
       <c r="AD3" s="36">
         <v>3.83</v>
       </c>
-      <c r="AE3" s="37">
+      <c r="AE3" s="41">
         <v>2656.22</v>
       </c>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
+      <c r="AF3" s="36">
+        <v>3.82</v>
+      </c>
+      <c r="AG3" s="37">
+        <v>2658.56</v>
+      </c>
       <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
     </row>
-    <row r="4" spans="1:35" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
@@ -7762,11 +8219,17 @@
       <c r="AD4" s="30">
         <v>3.71</v>
       </c>
-      <c r="AE4" s="26">
+      <c r="AE4" s="25">
         <v>2672.22</v>
       </c>
+      <c r="AF4" s="30">
+        <v>3.7</v>
+      </c>
+      <c r="AG4" s="26">
+        <v>2674.57</v>
+      </c>
     </row>
-    <row r="5" spans="1:35" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
@@ -7889,8 +8352,20 @@
         <f>(((AD3/365)*$B$6)/100)+AC5</f>
         <v>1.5109490410958906</v>
       </c>
+      <c r="AF5" s="38">
+        <f t="shared" ref="AF5" si="20">$B$5/AG3</f>
+        <v>0.36635770100695153</v>
+      </c>
+      <c r="AG5" s="39">
+        <f>(((AF3/365)*$B$6)/100)+AE5</f>
+        <v>1.6127808219178084</v>
+      </c>
+      <c r="AH5" s="47">
+        <f>AG5-E5</f>
+        <v>1.504018082191781</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>16</v>
       </c>
@@ -7917,7 +8392,7 @@
         <v>0.21192739726027399</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ref="H6" si="20">$B$6/I4</f>
+        <f t="shared" ref="H6" si="21">$B$6/I4</f>
         <v>0.36863042242849026</v>
       </c>
       <c r="I6" s="31">
@@ -7925,7 +8400,7 @@
         <v>0.31589178082191782</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6" si="21">$B$6/K4</f>
+        <f t="shared" ref="J6" si="22">$B$6/K4</f>
         <v>0.36872541514767965</v>
       </c>
       <c r="K6" s="31">
@@ -7933,7 +8408,7 @@
         <v>0.42012273972602743</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ref="L6" si="22">$B$6/M4</f>
+        <f t="shared" ref="L6" si="23">$B$6/M4</f>
         <v>0.37023930472635391</v>
       </c>
       <c r="M6" s="31">
@@ -7941,7 +8416,7 @@
         <v>0.52675287671232884</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6" si="23">$B$6/O4</f>
+        <f t="shared" ref="N6" si="24">$B$6/O4</f>
         <v>0.37126493358822027</v>
       </c>
       <c r="O6" s="31">
@@ -7949,7 +8424,7 @@
         <v>0.63498246575342476</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" ref="P6" si="24">$B$6/Q4</f>
+        <f t="shared" ref="P6" si="25">$B$6/Q4</f>
         <v>0.37061301602053798</v>
       </c>
       <c r="Q6" s="31">
@@ -7957,7 +8432,7 @@
         <v>0.74241232876712338</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" ref="R6" si="25">$B$6/S4</f>
+        <f t="shared" ref="R6" si="26">$B$6/S4</f>
         <v>0.36940576166684386</v>
       </c>
       <c r="S6" s="31">
@@ -7965,7 +8440,7 @@
         <v>0.84824273972602748</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" ref="T6" si="26">$B$6/U4</f>
+        <f t="shared" ref="T6" si="27">$B$6/U4</f>
         <v>0.37005625007131093</v>
       </c>
       <c r="U6" s="31">
@@ -7973,7 +8448,7 @@
         <v>0.95513945205479467</v>
       </c>
       <c r="V6" s="29">
-        <f t="shared" ref="V6" si="27">$B$6/W4</f>
+        <f t="shared" ref="V6" si="28">$B$6/W4</f>
         <v>0.36859969996817848</v>
       </c>
       <c r="W6" s="31">
@@ -7981,41 +8456,55 @@
         <v>1.0601701369863015</v>
       </c>
       <c r="X6" s="29">
-        <f t="shared" ref="X6" si="28">$B$6/Y4</f>
+        <f t="shared" ref="X6" si="29">$B$6/Y4</f>
         <v>0.36821610084504275</v>
       </c>
       <c r="Y6" s="31">
-        <f t="shared" ref="Y6" si="29">(((X4/365)*$B$6)/100)+W6</f>
+        <f t="shared" ref="Y6" si="30">(((X4/365)*$B$6)/100)+W6</f>
         <v>1.1646676712328767</v>
       </c>
       <c r="Z6" s="29">
-        <f t="shared" ref="Z6" si="30">$B$6/AA4</f>
+        <f t="shared" ref="Z6" si="31">$B$6/AA4</f>
         <v>0.36757900304112123</v>
       </c>
       <c r="AA6" s="31">
-        <f t="shared" ref="AA6" si="31">(((Z4/365)*$B$6)/100)+Y6</f>
+        <f t="shared" ref="AA6" si="32">(((Z4/365)*$B$6)/100)+Y6</f>
         <v>1.2683654794520549</v>
       </c>
       <c r="AB6" s="29">
-        <f t="shared" ref="AB6" si="32">$B$6/AC4</f>
+        <f t="shared" ref="AB6" si="33">$B$6/AC4</f>
         <v>0.36419713807675463</v>
       </c>
       <c r="AC6" s="31">
-        <f t="shared" ref="AC6" si="33">(((AB4/365)*$B$6)/100)+AA6</f>
+        <f t="shared" ref="AC6" si="34">(((AB4/365)*$B$6)/100)+AA6</f>
         <v>1.3672649315068495</v>
       </c>
       <c r="AD6" s="29">
-        <f t="shared" ref="AD6" si="34">$B$6/AE4</f>
+        <f t="shared" ref="AD6" si="35">$B$6/AE4</f>
         <v>0.36411672691619706</v>
       </c>
       <c r="AE6" s="31">
-        <f t="shared" ref="AE6" si="35">(((AD4/365)*$B$6)/100)+AC6</f>
+        <f t="shared" ref="AE6" si="36">(((AD4/365)*$B$6)/100)+AC6</f>
         <v>1.466164383561644</v>
       </c>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
-      <c r="AI6" s="22"/>
+      <c r="AF6" s="29">
+        <f t="shared" ref="AF6" si="37">$B$6/AG4</f>
+        <v>0.36379679724217351</v>
+      </c>
+      <c r="AG6" s="31">
+        <f t="shared" ref="AG6" si="38">(((AF4/365)*$B$6)/100)+AE6</f>
+        <v>1.5647972602739728</v>
+      </c>
+      <c r="AH6" s="47">
+        <f>AG6-E6</f>
+        <v>1.4592334246575345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AH7" s="48">
+        <f>AH5-AH6</f>
+        <v>4.4784657534246541E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 04/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LILIANE.xlsx
+++ b/TITULO COMPRADO - LILIANE.xlsx
@@ -901,8 +901,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-612754720"/>
-        <c:axId val="-612761792"/>
+        <c:axId val="-613864816"/>
+        <c:axId val="-613860464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1133,7 +1133,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -1353,7 +1353,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-612754720"/>
+        <c:axId val="-613864816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1396,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612761792"/>
+        <c:crossAx val="-613860464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1404,7 +1404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-612761792"/>
+        <c:axId val="-613860464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1455,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612754720"/>
+        <c:crossAx val="-613864816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2017,8 +2017,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-612762880"/>
-        <c:axId val="-612757984"/>
+        <c:axId val="-613859920"/>
+        <c:axId val="-613853936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2249,7 +2249,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$6</c15:sqref>
@@ -2469,7 +2469,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-612762880"/>
+        <c:axId val="-613859920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2512,7 +2512,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612757984"/>
+        <c:crossAx val="-613853936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2520,7 +2520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-612757984"/>
+        <c:axId val="-613853936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +2571,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612762880"/>
+        <c:crossAx val="-613859920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3133,8 +3133,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-612759072"/>
-        <c:axId val="-612765600"/>
+        <c:axId val="-613858832"/>
+        <c:axId val="-716501360"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3365,7 +3365,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -3585,7 +3585,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-612759072"/>
+        <c:axId val="-613858832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3628,7 +3628,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612765600"/>
+        <c:crossAx val="-716501360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3636,7 +3636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-612765600"/>
+        <c:axId val="-716501360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,7 +3687,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612759072"/>
+        <c:crossAx val="-613858832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4249,8 +4249,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-612753088"/>
-        <c:axId val="-612751456"/>
+        <c:axId val="-716498640"/>
+        <c:axId val="-716500816"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4481,7 +4481,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$4</c15:sqref>
@@ -4701,7 +4701,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-612753088"/>
+        <c:axId val="-716498640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4744,7 +4744,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612751456"/>
+        <c:crossAx val="-716500816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4752,7 +4752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-612751456"/>
+        <c:axId val="-716500816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4803,7 +4803,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612753088"/>
+        <c:crossAx val="-716498640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>